<commit_message>
Last update before transfer
</commit_message>
<xml_diff>
--- a/Zephyr_Test_Cases_Output.xlsx
+++ b/Zephyr_Test_Cases_Output.xlsx
@@ -888,8 +888,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is logged into the system, has access to the transaction list, and a filter is applied.
-The transaction list remains sorted and filtered as per the user's actions.</t>
+          <t>User is on the transaction list page with filters applied.
+Transaction list remains sorted and filtered as per user actions.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -986,8 +986,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is logged into the system, has access to the transaction list, and a filter is applied.
-The transaction list remains sorted and filtered as per the user's actions.</t>
+          <t>User is on the transaction list page with filters applied.
+Transaction list remains sorted and filtered as per user actions.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify the help guide is updated with filtering instructions</t>
+          <t>Verify help guide is updated with filtering instructions</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1189,13 +1189,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Navigate to the help guide section.</t>
+          <t>Open the help guide from the transaction list page.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Help guide is accessible and visible.</t>
+          <t>Help guide is displayed.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1210,8 +1210,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is logged into the system and has access to the help guide.
-User understands how to apply filters using the help guide.</t>
+          <t>User has access to the help guide.
+User is informed about filtering functionality through the help guide.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify the help guide is updated with filtering instructions</t>
+          <t>Verify help guide is updated with filtering instructions</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1308,8 +1308,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is logged into the system and has access to the help guide.
-User understands how to apply filters using the help guide.</t>
+          <t>User has access to the help guide.
+User is informed about filtering functionality through the help guide.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -1503,7 +1503,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Verify that the transaction graph does not refresh based on chosen filters</t>
+          <t>Verify that the transaction graph does not refresh based on the chosen filters</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1532,8 +1532,8 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>User is logged into the system, has access to the transaction list, and a filter is applied.
-The transaction graph remains static regardless of the filters applied to the list.</t>
+          <t>User is on the transaction list page with filters applied.
+Transaction graph remains static regardless of list filters.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Verify that the transaction graph does not refresh based on chosen filters</t>
+          <t>Verify that the transaction graph does not refresh based on the chosen filters</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -1615,7 +1615,7 @@
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>The transaction graph remains unchanged and does not reflect the applied filters.</t>
+          <t>The transaction graph remains unchanged and does not refresh based on the applied filters.</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -1630,8 +1630,8 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>User is logged into the system, has access to the transaction list, and a filter is applied.
-The transaction graph remains static regardless of the filters applied to the list.</t>
+          <t>User is on the transaction list page with filters applied.
+Transaction graph remains static regardless of list filters.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">

</xml_diff>